<commit_message>
Temp version to demo app
</commit_message>
<xml_diff>
--- a/Release/App/CheckList.xlsx
+++ b/Release/App/CheckList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\svi-quannguyen\Documents\GIT\iTools\Release\App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EC9640-5470-4767-8546-93ECE687C9B5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046A2BB0-664A-49F6-9FDE-4199F5E2A80A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8880" xr2:uid="{131CAA0E-2FFA-4783-9F10-C9546B25E973}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8880" xr2:uid="{131CAA0E-2FFA-4783-9F10-C9546B25E973}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="111">
   <si>
     <t>Login Page</t>
   </si>
@@ -747,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8750FA55-BA16-4A1D-B1AF-0B1568BF606F}">
   <dimension ref="A2:F183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,7 +1270,9 @@
       <c r="D41" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E41" s="3"/>
+      <c r="E41" s="3" t="s">
+        <v>110</v>
+      </c>
       <c r="F41" s="3"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1282,7 +1284,9 @@
       <c r="D42" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E42" s="3"/>
+      <c r="E42" s="3" t="s">
+        <v>110</v>
+      </c>
       <c r="F42" s="3"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1294,7 +1298,9 @@
       <c r="D43" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E43" s="3"/>
+      <c r="E43" s="3" t="s">
+        <v>110</v>
+      </c>
       <c r="F43" s="3"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1318,7 +1324,9 @@
       <c r="D45" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E45" s="3"/>
+      <c r="E45" s="3" t="s">
+        <v>110</v>
+      </c>
       <c r="F45" s="3"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>